<commit_message>
Updated plot with latest #s and regenerated plots for blog
</commit_message>
<xml_diff>
--- a/docs/plotting.xlsx
+++ b/docs/plotting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\documents\projects\cacheBenchmarker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\documents\projects\cacheBenchmarker\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{15D73814-75CD-45FC-A07D-6ADC939369A8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{83A387FA-08B1-4DCB-AB43-8932C1317214}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20310" windowHeight="7515" activeTab="1" xr2:uid="{A6AC2F04-4046-41A5-BA03-74AD473FDDFF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20310" windowHeight="7515" activeTab="2" xr2:uid="{A6AC2F04-4046-41A5-BA03-74AD473FDDFF}"/>
   </bookViews>
   <sheets>
     <sheet name="DELAYED_DURABILITY" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Disk Write</t>
   </si>
@@ -70,6 +70,18 @@
   <si>
     <t>Memory Select</t>
   </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Disk</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
 </sst>
 </file>
 
@@ -106,10 +118,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,22 +719,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>12605</c:v>
+                  <c:v>12546</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13762</c:v>
+                  <c:v>12511</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13870</c:v>
+                  <c:v>14040</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20098</c:v>
+                  <c:v>19216</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21742</c:v>
+                  <c:v>268683</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>373972</c:v>
+                  <c:v>294434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -988,7 +1000,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Redis vs SQL Server</a:t>
+              <a:t>SQL Server</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1102,32 +1114,29 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Reads writes sans get'!$A$3:$B$7</c:f>
+              <c:f>'Reads writes sans get'!$A$3:$B$6</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Disk Insert</c:v>
+                    <c:v>Insert</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Disk Select</c:v>
+                    <c:v>Select</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Memory Insert</c:v>
+                    <c:v>Insert</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Memory Select</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Set</c:v>
+                    <c:v>Select</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>SQL</c:v>
+                    <c:v>Disk</c:v>
                   </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Redis</c:v>
+                  <c:pt idx="2">
+                    <c:v>Memory</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1135,10 +1144,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Reads writes sans get'!$C$3:$C$7</c:f>
+              <c:f>'Reads writes sans get'!$C$3:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>12605</c:v>
                 </c:pt>
@@ -1150,9 +1159,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>20098</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3023,15 +3029,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:colOff>257174</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>114301</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>39053</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>65341</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3064,15 +3070,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>100011</xdr:rowOff>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>84390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3104,16 +3110,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3443,7 +3449,7 @@
   <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3453,7 +3459,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -3464,7 +3470,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -3473,7 +3479,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -3482,7 +3488,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -3491,7 +3497,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -3502,7 +3508,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -3511,7 +3517,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -3520,7 +3526,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -3542,8 +3548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4691A4-26F1-419A-AB36-7B2F1BCA6497}">
   <dimension ref="A3:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3552,76 +3558,76 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>12605</v>
+        <v>12546</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4">
-        <v>13762</v>
+        <v>12511</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>13870</v>
+        <v>14040</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6">
-        <v>20098</v>
+        <v>19216</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7">
-        <v>21742</v>
+        <v>268683</v>
       </c>
       <c r="D7">
         <f>C7/C5</f>
-        <v>1.5675558759913482</v>
+        <v>19.136965811965812</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8">
-        <v>373972</v>
+        <v>294434</v>
       </c>
       <c r="D8">
         <f>C8/C6</f>
-        <v>18.607423624241218</v>
+        <v>15.322335553705246</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3637,8 +3643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063DF525-8FED-4500-AF58-4C7D019ABCC0}">
   <dimension ref="A3:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3647,66 +3653,61 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
+      <c r="A3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>12605</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>13762</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>13870</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>20098</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>21742</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:A6"/>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>